<commit_message>
fixed the color for jcb and gs
..
</commit_message>
<xml_diff>
--- a/Convergence_of_Iterative_Methods/Convergence of iterative method data.xlsx
+++ b/Convergence_of_Iterative_Methods/Convergence of iterative method data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jihai\Desktop\Convergence_of_Iterative_Method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jihai\Desktop\AforAwful\Convergence_of_Iterative_Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,9 +49,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.0000000000000000000"/>
-    <numFmt numFmtId="171" formatCode="0.00000E+00"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -84,12 +84,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -221,14 +221,10 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:tint val="77000"/>
-                  </a:schemeClr>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -871,7 +867,7 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -1511,11 +1507,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="497595352"/>
-        <c:axId val="497591432"/>
+        <c:axId val="326819568"/>
+        <c:axId val="326821920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="497595352"/>
+        <c:axId val="326819568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,12 +1624,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497591432"/>
+        <c:crossAx val="326821920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="497591432"/>
+        <c:axId val="326821920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497595352"/>
+        <c:crossAx val="326819568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2662,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>